<commit_message>
cwa date change position
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340Process.xlsx
+++ b/DKS-API/Resources/Template/TempF340Process.xlsx
@@ -657,7 +657,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -752,11 +752,11 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>10</v>
@@ -845,10 +845,10 @@
         <v>37</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
F340 新增 PDMStatus 和 PDM Status Date
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempF340Process.xlsx
+++ b/DKS-API/Resources/Template/TempF340Process.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>HP系統</t>
   </si>
@@ -238,6 +238,22 @@
   </si>
   <si>
     <t>&amp;=result.CwaDeadline</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pdm Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pdm Status Date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.PdmStatus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=result.PdmStatusDate</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -265,7 +281,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +312,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -309,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,6 +357,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -651,13 +676,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -673,27 +698,27 @@
     <col min="10" max="10" width="34.28515625" style="5" customWidth="1"/>
     <col min="11" max="11" width="16.140625" style="5" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" style="5" customWidth="1"/>
-    <col min="13" max="14" width="20.42578125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" style="5" customWidth="1"/>
-    <col min="18" max="18" width="28" style="5" customWidth="1"/>
-    <col min="19" max="19" width="25.42578125" style="5" customWidth="1"/>
-    <col min="20" max="20" width="11" style="5" customWidth="1"/>
-    <col min="21" max="21" width="27.140625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="29" style="5" customWidth="1"/>
+    <col min="13" max="16" width="20.42578125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="5" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="5" customWidth="1"/>
+    <col min="20" max="20" width="28" style="5" customWidth="1"/>
+    <col min="21" max="21" width="25.42578125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="11" style="5" customWidth="1"/>
     <col min="23" max="23" width="27.140625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="25" style="5" customWidth="1"/>
-    <col min="25" max="25" width="24.85546875" style="5" customWidth="1"/>
-    <col min="26" max="26" width="25.5703125" style="5" customWidth="1"/>
+    <col min="24" max="24" width="29" style="5" customWidth="1"/>
+    <col min="25" max="25" width="27.140625" style="5" customWidth="1"/>
+    <col min="26" max="26" width="25" style="5" customWidth="1"/>
     <col min="27" max="27" width="24.85546875" style="5" customWidth="1"/>
-    <col min="28" max="28" width="15.5703125" style="5" customWidth="1"/>
-    <col min="29" max="29" width="25.140625" style="5" customWidth="1"/>
-    <col min="30" max="30" width="16" style="5" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="5"/>
+    <col min="28" max="28" width="25.5703125" style="5" customWidth="1"/>
+    <col min="29" max="29" width="24.85546875" style="5" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" style="5" customWidth="1"/>
+    <col min="31" max="31" width="25.140625" style="5" customWidth="1"/>
+    <col min="32" max="32" width="16" style="5" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -714,15 +739,15 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="8"/>
+      <c r="U1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
       <c r="V1" s="8"/>
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
@@ -732,8 +757,10 @@
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
       <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
     </row>
-    <row r="2" spans="1:30" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -776,56 +803,62 @@
       <c r="N2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -869,60 +902,66 @@
         <v>44</v>
       </c>
       <c r="O3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="V3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="Y3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="Z3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="AA3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AB3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AC3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AD3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AC3" s="5" t="s">
+      <c r="AE3" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AD3" s="5" t="s">
+      <c r="AF3" s="5" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:AD1"/>
+    <mergeCell ref="D1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:AF1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>